<commit_message>
LIRV notes & Tute 3
</commit_message>
<xml_diff>
--- a/LIRV/Textbook/LI&R Valuation S1 2020 M05 Table 5.2 IBNR Chain Ladder.xlsx
+++ b/LIRV/Textbook/LI&R Valuation S1 2020 M05 Table 5.2 IBNR Chain Ladder.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\STRATEGIC PROJECTS OFFICE\Education Strategy 2018-2022\Course development\Fellowship Modules\LIaR Modules\LIaR Valuation\2018 Development\Module 5 LI liability valuation methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VZhu\Documents\GitHub\my_file\LIRV\Textbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{65403B77-AF8E-492F-A1BF-6C0C1E8AA648}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" activeTab="3" xr2:uid="{CAB0F408-F3B7-42ED-AAD5-E3A2A3F5E102}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="3" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Calculations" sheetId="2" r:id="rId3"/>
     <sheet name="Tables" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,12 +27,46 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Vincent Zhu</author>
+  </authors>
+  <commentList>
+    <comment ref="D19" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vincent Zhu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Average development factor for the period from month 1 to month 12 is not used, as the relatively small number of claims reported during the year of incidence makes this ratio quite volatile.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam A</author>
   </authors>
   <commentList>
-    <comment ref="D28" authorId="0" shapeId="0" xr:uid="{EEE98434-B078-41A3-9E3B-B935596DB4A8}">
+    <comment ref="D28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -179,12 +212,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00,;\(#,##0.00,\);0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +291,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="0.79998168889431442"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +345,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,7 +739,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -696,15 +754,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -759,12 +808,6 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -793,15 +836,6 @@
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -839,9 +873,6 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -874,36 +905,12 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1013,12 +1020,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1050,6 +1051,66 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1364,7 +1425,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD07CC9-B6F6-4BE8-AC09-E1E235C0DD1A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1374,7 +1435,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="79" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1404,17 +1465,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5364F000-769A-42FD-A379-309696E6E6DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:S60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="2" customWidth="1"/>
-    <col min="2" max="4" width="10.7109375" style="79"/>
+    <col min="2" max="4" width="10.7109375" style="70"/>
     <col min="5" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
@@ -1426,15 +1487,15 @@
       <c r="D2" s="1"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="141" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
-      <c r="H4" s="93"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="141"/>
     </row>
     <row r="5" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
@@ -1455,344 +1516,344 @@
     <row r="6" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="143"/>
+      <c r="I6" s="143"/>
+      <c r="J6" s="143"/>
+      <c r="K6" s="144"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
     </row>
     <row r="7" spans="2:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>0</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="11">
         <v>12</v>
       </c>
-      <c r="F7" s="14">
-        <f>E7+12</f>
+      <c r="F7" s="11">
+        <f t="shared" ref="F7:K7" si="0">E7+12</f>
         <v>24</v>
       </c>
-      <c r="G7" s="14">
-        <f>F7+12</f>
+      <c r="G7" s="11">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="H7" s="14">
-        <f>G7+12</f>
+      <c r="H7" s="11">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="I7" s="14">
-        <f>H7+12</f>
+      <c r="I7" s="11">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="J7" s="14">
-        <f>I7+12</f>
+      <c r="J7" s="11">
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="K7" s="15">
-        <f>J7+12</f>
+      <c r="K7" s="12">
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="L7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
+      <c r="L7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="20"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="21"/>
+      <c r="M8" s="18"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
     </row>
     <row r="9" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>2010</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="20">
         <v>60124.691358024691</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <v>3330.86</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="21">
         <v>12811</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="21">
         <v>20370</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="21">
         <v>26656</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="21">
         <v>37667</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="21">
         <v>44414</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="21">
         <v>48701</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="22">
         <v>48701</v>
       </c>
       <c r="L9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="26"/>
+      <c r="P9" s="23"/>
     </row>
     <row r="10" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="27">
-        <f>B9+1</f>
+      <c r="B10" s="24">
+        <f t="shared" ref="B10:B16" si="1">B9+1</f>
         <v>2011</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="20">
         <v>65235.290123456791</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <v>1447.6499999999999</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <v>9651</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="21">
         <v>16995</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <v>30354</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <v>40594</v>
       </c>
-      <c r="I10" s="24">
+      <c r="I10" s="21">
         <v>44231</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="21">
         <v>44373</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="22"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="29"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="26"/>
     </row>
     <row r="11" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="27">
-        <f>B10+1</f>
+      <c r="B11" s="24">
+        <f t="shared" si="1"/>
         <v>2012</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="20">
         <v>75281.524802469125</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <v>1529.55</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="21">
         <v>16995</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="21">
         <v>40180</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="21">
         <v>58866</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="21">
         <v>71707</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="21">
         <f>H11</f>
         <v>71707</v>
       </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
       <c r="L11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="29"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="26"/>
     </row>
     <row r="12" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="27">
-        <f>B11+1</f>
+      <c r="B12" s="24">
+        <f t="shared" si="1"/>
         <v>2013</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>78970.319517790107</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="21">
         <v>5161.32</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="21">
         <v>28674</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="21">
         <v>47432</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="21">
         <v>70340</v>
       </c>
-      <c r="H12" s="24">
+      <c r="H12" s="21">
         <v>71690</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="29"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="26"/>
     </row>
     <row r="13" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="27">
-        <f>B12+1</f>
+      <c r="B13" s="24">
+        <f t="shared" si="1"/>
         <v>2014</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="20">
         <v>80154.874310556945</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="21">
         <v>6225.18</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="21">
         <v>27066</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="21">
         <v>46783</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="21">
         <v>48804</v>
       </c>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="29"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="26"/>
     </row>
     <row r="14" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27">
-        <f>B13+1</f>
+      <c r="B14" s="24">
+        <f t="shared" si="1"/>
         <v>2015</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="20">
         <v>76948.679338134665</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="21">
         <v>4325</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="21">
         <v>19477</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="21">
         <v>31732</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="25"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="22"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
     </row>
     <row r="15" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27">
-        <f>B14+1</f>
+      <c r="B15" s="24">
+        <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="20">
         <v>75409.705751371977</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="21">
         <v>931.6</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="21">
         <v>18632</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
     </row>
     <row r="16" spans="2:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="30">
-        <f>B15+1</f>
+      <c r="B16" s="27">
+        <f t="shared" si="1"/>
         <v>2017</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="28">
         <v>77294.948395156272</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="29">
         <v>2232</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="33"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="30"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
     </row>
     <row r="17" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
@@ -1848,11 +1909,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520F152B-EF54-429D-BBCB-66A6F930116E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:D55"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1871,28 +1932,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="79" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="79" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38"/>
+      <c r="D3" s="145"/>
+      <c r="E3" s="145"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="146"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
@@ -1903,40 +1964,40 @@
       <c r="R3" s="2"/>
     </row>
     <row r="4" spans="1:18" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>0</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>12</v>
       </c>
-      <c r="E4" s="14">
-        <f>D4+12</f>
+      <c r="E4" s="11">
+        <f t="shared" ref="E4:J4" si="0">D4+12</f>
         <v>24</v>
       </c>
-      <c r="F4" s="14">
-        <f>E4+12</f>
+      <c r="F4" s="11">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="G4" s="14">
-        <f>F4+12</f>
+      <c r="G4" s="11">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="H4" s="14">
-        <f>G4+12</f>
+      <c r="H4" s="11">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="I4" s="14">
-        <f>H4+12</f>
+      <c r="I4" s="11">
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="J4" s="15">
-        <f>I4+12</f>
+      <c r="J4" s="12">
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
       <c r="K4" s="5"/>
@@ -1949,16 +2010,16 @@
       <c r="R4" s="2"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="41"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="36"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -1969,40 +2030,40 @@
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="42">
+      <c r="A6" s="37">
         <f>Data!B9</f>
         <v>2010</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="20">
         <f>Data!C9</f>
         <v>60124.691358024691</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44">
+      <c r="C6" s="38"/>
+      <c r="D6" s="39">
         <f>Data!E9/Data!D9</f>
         <v>3.8461538461538458</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="39">
         <f>Data!F9/Data!E9</f>
         <v>1.5900398095386776</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="39">
         <f>Data!G9/Data!F9</f>
         <v>1.3085910652920962</v>
       </c>
-      <c r="G6" s="44">
+      <c r="G6" s="39">
         <f>Data!H9/Data!G9</f>
         <v>1.413077731092437</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="39">
         <f>Data!I9/Data!H9</f>
         <v>1.1791223086521359</v>
       </c>
-      <c r="I6" s="44">
+      <c r="I6" s="39">
         <f>Data!J9/Data!I9</f>
         <v>1.096523618678795</v>
       </c>
-      <c r="J6" s="45">
+      <c r="J6" s="40">
         <f>Data!K9/Data!J9</f>
         <v>1</v>
       </c>
@@ -2016,40 +2077,40 @@
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="42">
-        <f>A6+1</f>
+      <c r="A7" s="37">
+        <f t="shared" ref="A7:A13" si="1">A6+1</f>
         <v>2011</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="20">
         <f>Data!C10</f>
         <v>65235.290123456791</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="44">
+      <c r="C7" s="41"/>
+      <c r="D7" s="39">
         <f>Data!E10/Data!D10</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="39">
         <f>Data!F10/Data!E10</f>
         <v>1.7609574137395088</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="39">
         <f>Data!G10/Data!F10</f>
         <v>1.7860547219770522</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="39">
         <f>Data!H10/Data!G10</f>
         <v>1.3373525729722606</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="39">
         <f>Data!I10/Data!H10</f>
         <v>1.0895945213578362</v>
       </c>
-      <c r="I7" s="44">
+      <c r="I7" s="39">
         <f>Data!J10/Data!I10</f>
         <v>1.0032104180326016</v>
       </c>
-      <c r="J7" s="45"/>
+      <c r="J7" s="40"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -2060,37 +2121,37 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="42">
-        <f>A7+1</f>
+      <c r="A8" s="37">
+        <f t="shared" si="1"/>
         <v>2012</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="20">
         <f>Data!C11</f>
         <v>75281.524802469125</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="44">
+      <c r="C8" s="41"/>
+      <c r="D8" s="39">
         <f>Data!E11/Data!D11</f>
         <v>11.111111111111111</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="39">
         <f>Data!F11/Data!E11</f>
         <v>2.3642247719917622</v>
       </c>
-      <c r="F8" s="44">
+      <c r="F8" s="39">
         <f>Data!G11/Data!F11</f>
         <v>1.4650572424091588</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="39">
         <f>Data!H11/Data!G11</f>
         <v>1.2181395032786329</v>
       </c>
-      <c r="H8" s="44">
+      <c r="H8" s="39">
         <f>Data!I11/Data!H11</f>
         <v>1</v>
       </c>
-      <c r="I8" s="44"/>
-      <c r="J8" s="45"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -2101,34 +2162,34 @@
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="42">
-        <f>A8+1</f>
+      <c r="A9" s="37">
+        <f t="shared" si="1"/>
         <v>2013</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="20">
         <f>Data!C12</f>
         <v>78970.319517790107</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="44">
+      <c r="C9" s="41"/>
+      <c r="D9" s="39">
         <f>Data!E12/Data!D12</f>
         <v>5.5555555555555562</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="39">
         <f>Data!F12/Data!E12</f>
         <v>1.6541814884564414</v>
       </c>
-      <c r="F9" s="44">
+      <c r="F9" s="39">
         <f>Data!G12/Data!F12</f>
         <v>1.4829650868611908</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="39">
         <f>Data!H12/Data!G12</f>
         <v>1.0191924936025021</v>
       </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="45"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -2139,31 +2200,31 @@
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="42">
-        <f>A9+1</f>
+      <c r="A10" s="37">
+        <f t="shared" si="1"/>
         <v>2014</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="20">
         <f>Data!C13</f>
         <v>80154.874310556945</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="44">
+      <c r="C10" s="41"/>
+      <c r="D10" s="39">
         <f>Data!E13/Data!D13</f>
         <v>4.3478260869565215</v>
       </c>
-      <c r="E10" s="44">
+      <c r="E10" s="39">
         <f>Data!F13/Data!E13</f>
         <v>1.7284785339540383</v>
       </c>
-      <c r="F10" s="44">
+      <c r="F10" s="39">
         <f>Data!G13/Data!F13</f>
         <v>1.0431994527926811</v>
       </c>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="45"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -2174,28 +2235,28 @@
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="42">
-        <f>A10+1</f>
+      <c r="A11" s="37">
+        <f t="shared" si="1"/>
         <v>2015</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="20">
         <f>Data!C14</f>
         <v>76948.679338134665</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="44">
+      <c r="C11" s="41"/>
+      <c r="D11" s="39">
         <f>Data!E14/Data!D14</f>
         <v>4.5033526011560694</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="39">
         <f>Data!F14/Data!E14</f>
         <v>1.6292036761308211</v>
       </c>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="45"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -2206,26 +2267,26 @@
       <c r="R11" s="2"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="42">
-        <f>A11+1</f>
+      <c r="A12" s="37">
+        <f t="shared" si="1"/>
         <v>2016</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="20">
         <f>Data!C15</f>
         <v>75409.705751371977</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="44">
+      <c r="C12" s="41"/>
+      <c r="D12" s="39">
         <f>Data!E15/Data!D15</f>
         <v>20</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="24"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="21"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
@@ -2235,23 +2296,23 @@
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="42">
-        <f>A12+1</f>
+      <c r="A13" s="37">
+        <f t="shared" si="1"/>
         <v>2017</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="20">
         <f>Data!C16</f>
         <v>77294.948395156272</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="24"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -2261,16 +2322,16 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
+      <c r="A14" s="37"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="22"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -2281,41 +2342,41 @@
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49">
-        <f>AVERAGE(D6:D12)</f>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44">
+        <f t="shared" ref="D15:J15" si="2">AVERAGE(D6:D12)</f>
         <v>8.0043808382285384</v>
       </c>
-      <c r="E15" s="49">
-        <f>AVERAGE(E6:E12)</f>
+      <c r="E15" s="44">
+        <f t="shared" si="2"/>
         <v>1.7878476156352086</v>
       </c>
-      <c r="F15" s="49">
-        <f>AVERAGE(F6:F12)</f>
+      <c r="F15" s="44">
+        <f t="shared" si="2"/>
         <v>1.4171735138664356</v>
       </c>
-      <c r="G15" s="49">
-        <f>AVERAGE(G6:G12)</f>
+      <c r="G15" s="44">
+        <f t="shared" si="2"/>
         <v>1.2469405752364582</v>
       </c>
-      <c r="H15" s="49">
-        <f>AVERAGE(H6:H12)</f>
+      <c r="H15" s="44">
+        <f t="shared" si="2"/>
         <v>1.0895722766699907</v>
       </c>
-      <c r="I15" s="49">
-        <f>AVERAGE(I6:I12)</f>
+      <c r="I15" s="44">
+        <f t="shared" si="2"/>
         <v>1.0498670183556982</v>
       </c>
-      <c r="J15" s="49">
-        <f>AVERAGE(J6:J12)</f>
+      <c r="J15" s="44">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K15" s="5"/>
-      <c r="L15" s="46"/>
+      <c r="L15" s="41"/>
       <c r="M15" s="2"/>
       <c r="N15" s="5"/>
       <c r="O15" s="2"/>
@@ -2324,20 +2385,20 @@
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
       <c r="K16" s="5"/>
-      <c r="L16" s="46"/>
+      <c r="L16" s="41"/>
       <c r="M16" s="2"/>
       <c r="N16" s="5"/>
       <c r="O16" s="2"/>
@@ -2346,18 +2407,18 @@
       <c r="R16" s="2"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="46"/>
+      <c r="L17" s="41"/>
       <c r="M17" s="2"/>
       <c r="N17" s="5"/>
       <c r="O17" s="2"/>
@@ -2366,44 +2427,44 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="48">
-        <f>C4</f>
+      <c r="B18" s="147"/>
+      <c r="C18" s="43">
+        <f t="shared" ref="C18:J18" si="3">C4</f>
         <v>0</v>
       </c>
-      <c r="D18" s="48">
-        <f>D4</f>
+      <c r="D18" s="43">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="E18" s="48">
-        <f>E4</f>
+      <c r="E18" s="43">
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="F18" s="48">
-        <f>F4</f>
+      <c r="F18" s="43">
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="G18" s="48">
-        <f>G4</f>
+      <c r="G18" s="43">
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="H18" s="48">
-        <f>H4</f>
+      <c r="H18" s="43">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="I18" s="48">
-        <f>I4</f>
+      <c r="I18" s="43">
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="J18" s="48">
-        <f>J4</f>
+      <c r="J18" s="43">
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
       <c r="K18" s="5"/>
-      <c r="L18" s="46"/>
+      <c r="L18" s="41"/>
       <c r="M18" s="2"/>
       <c r="N18" s="5"/>
       <c r="O18" s="2"/>
@@ -2412,44 +2473,44 @@
       <c r="R18" s="2"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="51" t="s">
+      <c r="A19" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="52"/>
-      <c r="C19" s="48">
-        <f>C15</f>
+      <c r="B19" s="149"/>
+      <c r="C19" s="43">
+        <f t="shared" ref="C19:J19" si="4">C15</f>
         <v>0</v>
       </c>
-      <c r="D19" s="53">
-        <f>D15</f>
+      <c r="D19" s="45">
+        <f t="shared" si="4"/>
         <v>8.0043808382285384</v>
       </c>
-      <c r="E19" s="53">
-        <f>E15</f>
+      <c r="E19" s="160">
+        <f t="shared" si="4"/>
         <v>1.7878476156352086</v>
       </c>
-      <c r="F19" s="53">
-        <f>F15</f>
+      <c r="F19" s="160">
+        <f t="shared" si="4"/>
         <v>1.4171735138664356</v>
       </c>
-      <c r="G19" s="53">
-        <f>G15</f>
+      <c r="G19" s="160">
+        <f t="shared" si="4"/>
         <v>1.2469405752364582</v>
       </c>
-      <c r="H19" s="53">
-        <f>H15</f>
+      <c r="H19" s="160">
+        <f t="shared" si="4"/>
         <v>1.0895722766699907</v>
       </c>
-      <c r="I19" s="53">
-        <f>I15</f>
+      <c r="I19" s="160">
+        <f t="shared" si="4"/>
         <v>1.0498670183556982</v>
       </c>
-      <c r="J19" s="53">
-        <f>J15</f>
+      <c r="J19" s="160">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K19" s="5"/>
-      <c r="L19" s="46"/>
+      <c r="L19" s="41"/>
       <c r="M19" s="2"/>
       <c r="N19" s="5"/>
       <c r="O19" s="2"/>
@@ -2458,18 +2519,18 @@
       <c r="R19" s="2"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
       <c r="K20" s="5"/>
-      <c r="L20" s="46"/>
+      <c r="L20" s="41"/>
       <c r="M20" s="2"/>
       <c r="N20" s="5"/>
       <c r="O20" s="2"/>
@@ -2478,42 +2539,42 @@
       <c r="R20" s="2"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
-      <c r="B21" s="46"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="2">
         <f>Data!B9</f>
         <v>2010</v>
       </c>
       <c r="D21" s="2">
-        <f>C21+1</f>
+        <f t="shared" ref="D21:J21" si="5">C21+1</f>
         <v>2011</v>
       </c>
       <c r="E21" s="2">
-        <f>D21+1</f>
+        <f t="shared" si="5"/>
         <v>2012</v>
       </c>
       <c r="F21" s="2">
-        <f>E21+1</f>
+        <f t="shared" si="5"/>
         <v>2013</v>
       </c>
       <c r="G21" s="2">
-        <f>F21+1</f>
+        <f t="shared" si="5"/>
         <v>2014</v>
       </c>
       <c r="H21" s="2">
-        <f>G21+1</f>
+        <f t="shared" si="5"/>
         <v>2015</v>
       </c>
       <c r="I21" s="2">
-        <f>H21+1</f>
+        <f t="shared" si="5"/>
         <v>2016</v>
       </c>
       <c r="J21" s="2">
-        <f>I21+1</f>
+        <f t="shared" si="5"/>
         <v>2017</v>
       </c>
       <c r="K21" s="5"/>
-      <c r="L21" s="46"/>
+      <c r="L21" s="41"/>
       <c r="M21" s="2"/>
       <c r="N21" s="5"/>
       <c r="O21" s="2"/>
@@ -2522,42 +2583,42 @@
       <c r="R21" s="2"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="54">
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="46">
         <v>0</v>
       </c>
-      <c r="D22" s="55">
-        <f>C22+12</f>
+      <c r="D22" s="47">
+        <f t="shared" ref="D22:J22" si="6">C22+12</f>
         <v>12</v>
       </c>
-      <c r="E22" s="55">
-        <f>D22+12</f>
+      <c r="E22" s="47">
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="F22" s="55">
-        <f>E22+12</f>
+      <c r="F22" s="47">
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
-      <c r="G22" s="55">
-        <f>F22+12</f>
+      <c r="G22" s="47">
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
-      <c r="H22" s="55">
-        <f>G22+12</f>
+      <c r="H22" s="47">
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="I22" s="55">
-        <f>H22+12</f>
+      <c r="I22" s="47">
+        <f t="shared" si="6"/>
         <v>72</v>
       </c>
-      <c r="J22" s="55">
-        <f>I22+12</f>
+      <c r="J22" s="47">
+        <f t="shared" si="6"/>
         <v>84</v>
       </c>
       <c r="K22" s="5"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="46"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
       <c r="N22" s="5"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -2565,21 +2626,21 @@
       <c r="R22" s="2"/>
     </row>
     <row r="23" spans="1:18" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="90" t="s">
+      <c r="A23" s="48"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="89"/>
+      <c r="D23" s="151"/>
+      <c r="E23" s="151"/>
+      <c r="F23" s="151"/>
+      <c r="G23" s="151"/>
+      <c r="H23" s="151"/>
+      <c r="I23" s="151"/>
+      <c r="J23" s="152"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="46"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
       <c r="N23" s="5"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -2587,98 +2648,98 @@
       <c r="R23" s="2"/>
     </row>
     <row r="24" spans="1:18" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="9">
         <v>0</v>
       </c>
-      <c r="D24" s="14">
-        <f>C24+12</f>
+      <c r="D24" s="11">
+        <f t="shared" ref="D24:J24" si="7">C24+12</f>
         <v>12</v>
       </c>
-      <c r="E24" s="14">
-        <f>D24+12</f>
+      <c r="E24" s="11">
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="F24" s="14">
-        <f>E24+12</f>
+      <c r="F24" s="11">
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
-      <c r="G24" s="14">
-        <f>F24+12</f>
+      <c r="G24" s="11">
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
-      <c r="H24" s="14">
-        <f>G24+12</f>
+      <c r="H24" s="11">
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="I24" s="14">
-        <f>H24+12</f>
+      <c r="I24" s="11">
+        <f t="shared" si="7"/>
         <v>72</v>
       </c>
-      <c r="J24" s="15">
-        <f>I24+12</f>
+      <c r="J24" s="12">
+        <f t="shared" si="7"/>
         <v>84</v>
       </c>
       <c r="K24" s="2"/>
       <c r="R24" s="2"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="41"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="36"/>
       <c r="K25" s="2"/>
       <c r="R25" s="2"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
+      <c r="A26" s="24">
         <f>Data!B9</f>
         <v>2010</v>
       </c>
-      <c r="B26" s="23">
+      <c r="B26" s="20">
         <f>Data!C9</f>
         <v>60124.691358024691</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="21">
         <f>Data!D9</f>
         <v>3330.86</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="21">
         <f>Data!E9</f>
         <v>12811</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="21">
         <f>Data!F9</f>
         <v>20370</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="21">
         <f>Data!G9</f>
         <v>26656</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="21">
         <f>Data!H9</f>
         <v>37667</v>
       </c>
-      <c r="H26" s="24">
+      <c r="H26" s="21">
         <f>Data!I9</f>
         <v>44414</v>
       </c>
-      <c r="I26" s="24">
+      <c r="I26" s="21">
         <f>Data!J9</f>
         <v>48701</v>
       </c>
-      <c r="J26" s="25">
+      <c r="J26" s="22">
         <f>Data!K9</f>
         <v>48701</v>
       </c>
@@ -2686,307 +2747,307 @@
       <c r="R26" s="2"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="42">
-        <f>A26+1</f>
+      <c r="A27" s="37">
+        <f t="shared" ref="A27:A33" si="8">A26+1</f>
         <v>2011</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B27" s="20">
         <f>Data!C10</f>
         <v>65235.290123456791</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="21">
         <f>Data!D10</f>
         <v>1447.6499999999999</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="21">
         <f>Data!E10</f>
         <v>9651</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="21">
         <f>Data!F10</f>
         <v>16995</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="21">
         <f>Data!G10</f>
         <v>30354</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="21">
         <f>Data!H10</f>
         <v>40594</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="21">
         <f>Data!I10</f>
         <v>44231</v>
       </c>
-      <c r="I27" s="24">
+      <c r="I27" s="21">
         <f>Data!J10</f>
         <v>44373</v>
       </c>
-      <c r="J27" s="65">
-        <f>I27*J$19</f>
+      <c r="J27" s="57">
+        <f t="shared" ref="J27:J32" si="9">I27*J$19</f>
         <v>44373</v>
       </c>
       <c r="K27" s="2"/>
       <c r="R27" s="2"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="42">
-        <f>A27+1</f>
+      <c r="A28" s="37">
+        <f t="shared" si="8"/>
         <v>2012</v>
       </c>
-      <c r="B28" s="23">
+      <c r="B28" s="20">
         <f>Data!C11</f>
         <v>75281.524802469125</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="21">
         <f>Data!D11</f>
         <v>1529.55</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="21">
         <f>Data!E11</f>
         <v>16995</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="21">
         <f>Data!F11</f>
         <v>40180</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28" s="21">
         <f>Data!G11</f>
         <v>58866</v>
       </c>
-      <c r="G28" s="24">
+      <c r="G28" s="21">
         <f>Data!H11</f>
         <v>71707</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="21">
         <f>Data!I11</f>
         <v>71707</v>
       </c>
-      <c r="I28" s="66">
+      <c r="I28" s="58">
         <f>H28*I$19</f>
         <v>75282.814285232045</v>
       </c>
-      <c r="J28" s="65">
-        <f>I28*J$19</f>
+      <c r="J28" s="57">
+        <f t="shared" si="9"/>
         <v>75282.814285232045</v>
       </c>
       <c r="K28" s="2"/>
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="42">
-        <f>A28+1</f>
+      <c r="A29" s="37">
+        <f t="shared" si="8"/>
         <v>2013</v>
       </c>
-      <c r="B29" s="23">
+      <c r="B29" s="20">
         <f>Data!C12</f>
         <v>78970.319517790107</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="21">
         <f>Data!D12</f>
         <v>5161.32</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="21">
         <f>Data!E12</f>
         <v>28674</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="21">
         <f>Data!F12</f>
         <v>47432</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="21">
         <f>Data!G12</f>
         <v>70340</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="21">
         <f>Data!H12</f>
         <v>71690</v>
       </c>
-      <c r="H29" s="66">
+      <c r="H29" s="58">
         <f>G29*H$19</f>
         <v>78111.436514471628</v>
       </c>
-      <c r="I29" s="66">
+      <c r="I29" s="58">
         <f>H29*I$19</f>
         <v>82006.620952928744</v>
       </c>
-      <c r="J29" s="65">
-        <f>I29*J$19</f>
+      <c r="J29" s="57">
+        <f t="shared" si="9"/>
         <v>82006.620952928744</v>
       </c>
       <c r="K29" s="2"/>
       <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="42">
-        <f>A29+1</f>
+      <c r="A30" s="37">
+        <f t="shared" si="8"/>
         <v>2014</v>
       </c>
-      <c r="B30" s="23">
+      <c r="B30" s="20">
         <f>Data!C13</f>
         <v>80154.874310556945</v>
       </c>
-      <c r="C30" s="24">
+      <c r="C30" s="21">
         <f>Data!D13</f>
         <v>6225.18</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="21">
         <f>Data!E13</f>
         <v>27066</v>
       </c>
-      <c r="E30" s="24">
+      <c r="E30" s="21">
         <f>Data!F13</f>
         <v>46783</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="21">
         <f>Data!G13</f>
         <v>48804</v>
       </c>
-      <c r="G30" s="66">
+      <c r="G30" s="58">
         <f>F30*G$19</f>
         <v>60855.687833840107</v>
       </c>
-      <c r="H30" s="66">
+      <c r="H30" s="58">
         <f>G30*H$19</f>
         <v>66306.670341435412</v>
       </c>
-      <c r="I30" s="66">
+      <c r="I30" s="58">
         <f>H30*I$19</f>
         <v>69613.186288457</v>
       </c>
-      <c r="J30" s="65">
-        <f>I30*J$19</f>
+      <c r="J30" s="57">
+        <f t="shared" si="9"/>
         <v>69613.186288457</v>
       </c>
       <c r="K30" s="2"/>
       <c r="R30" s="2"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="42">
-        <f>A30+1</f>
+      <c r="A31" s="37">
+        <f t="shared" si="8"/>
         <v>2015</v>
       </c>
-      <c r="B31" s="23">
+      <c r="B31" s="20">
         <f>Data!C14</f>
         <v>76948.679338134665</v>
       </c>
-      <c r="C31" s="24">
+      <c r="C31" s="21">
         <f>Data!D14</f>
         <v>4325</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="21">
         <f>Data!E14</f>
         <v>19477</v>
       </c>
-      <c r="E31" s="24">
+      <c r="E31" s="21">
         <f>Data!F14</f>
         <v>31732</v>
       </c>
-      <c r="F31" s="66">
+      <c r="F31" s="58">
         <f>E31*F$19</f>
         <v>44969.749942009737</v>
       </c>
-      <c r="G31" s="66">
+      <c r="G31" s="58">
         <f>F31*G$19</f>
         <v>56074.605860929303</v>
       </c>
-      <c r="H31" s="66">
+      <c r="H31" s="58">
         <f>G31*H$19</f>
         <v>61097.335971265144</v>
       </c>
-      <c r="I31" s="66">
+      <c r="I31" s="58">
         <f>H31*I$19</f>
         <v>64144.07794562848</v>
       </c>
-      <c r="J31" s="65">
-        <f>I31*J$19</f>
+      <c r="J31" s="57">
+        <f t="shared" si="9"/>
         <v>64144.07794562848</v>
       </c>
       <c r="K31" s="2"/>
       <c r="R31" s="2"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="42">
-        <f>A31+1</f>
+      <c r="A32" s="37">
+        <f t="shared" si="8"/>
         <v>2016</v>
       </c>
-      <c r="B32" s="23">
+      <c r="B32" s="20">
         <f>Data!C15</f>
         <v>75409.705751371977</v>
       </c>
-      <c r="C32" s="24">
+      <c r="C32" s="21">
         <f>Data!D15</f>
         <v>931.6</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="21">
         <f>Data!E15</f>
         <v>18632</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="58">
         <f>D32*E$19</f>
         <v>33311.176774515203</v>
       </c>
-      <c r="F32" s="66">
+      <c r="F32" s="58">
         <f>E32*F$19</f>
         <v>47207.717440565713</v>
       </c>
-      <c r="G32" s="66">
+      <c r="G32" s="58">
         <f>F32*G$19</f>
         <v>58865.218340939187</v>
       </c>
-      <c r="H32" s="66">
+      <c r="H32" s="58">
         <f>G32*H$19</f>
         <v>64137.9099644132</v>
       </c>
-      <c r="I32" s="66">
+      <c r="I32" s="58">
         <f>H32*I$19</f>
         <v>67336.276297904711</v>
       </c>
-      <c r="J32" s="65">
-        <f>I32*J$19</f>
+      <c r="J32" s="57">
+        <f t="shared" si="9"/>
         <v>67336.276297904711</v>
       </c>
       <c r="K32" s="2"/>
       <c r="R32" s="2"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="42">
-        <f>A32+1</f>
+      <c r="A33" s="37">
+        <f t="shared" si="8"/>
         <v>2017</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="20">
         <f>Data!C16</f>
         <v>77294.948395156272</v>
       </c>
-      <c r="C33" s="24">
+      <c r="C33" s="21">
         <f>Data!D16</f>
         <v>2232</v>
       </c>
-      <c r="D33" s="66">
-        <f>E33/E19</f>
+      <c r="D33" s="58">
+        <f t="shared" ref="D33:I33" si="10">E33/E19</f>
         <v>18853.926499115285</v>
       </c>
-      <c r="E33" s="66">
-        <f>F33/F19</f>
+      <c r="E33" s="58">
+        <f t="shared" si="10"/>
         <v>33707.947536804735</v>
       </c>
-      <c r="F33" s="66">
-        <f>G33/G19</f>
+      <c r="F33" s="58">
+        <f t="shared" si="10"/>
         <v>47770.010455959025</v>
       </c>
-      <c r="G33" s="66">
-        <f>H33/H19</f>
+      <c r="G33" s="58">
+        <f t="shared" si="10"/>
         <v>59566.364317005166</v>
       </c>
-      <c r="H33" s="66">
-        <f>I33/I19</f>
+      <c r="H33" s="58">
+        <f t="shared" si="10"/>
         <v>64901.85918183341</v>
       </c>
-      <c r="I33" s="66">
-        <f>J33/J19</f>
+      <c r="I33" s="58">
+        <f t="shared" si="10"/>
         <v>68138.321384972834</v>
       </c>
-      <c r="J33" s="65">
+      <c r="J33" s="57">
         <f>E54+C33</f>
         <v>68138.321384972834</v>
       </c>
@@ -2994,50 +3055,50 @@
       <c r="R33" s="2"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="72"/>
+      <c r="J34" s="64"/>
       <c r="K34" s="2"/>
       <c r="R34" s="2"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="77" t="s">
+      <c r="A35" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="78"/>
-      <c r="D35" s="32">
+      <c r="B35" s="27"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="29">
         <f>D33</f>
         <v>18853.926499115285</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="29">
         <f>SUM(E32:E33)</f>
         <v>67019.124311319931</v>
       </c>
-      <c r="F35" s="32">
+      <c r="F35" s="29">
         <f>SUM(F31:F33)</f>
         <v>139947.47783853445</v>
       </c>
-      <c r="G35" s="32">
+      <c r="G35" s="29">
         <f>SUM(G30:G33)</f>
         <v>235361.87635271373</v>
       </c>
-      <c r="H35" s="32">
+      <c r="H35" s="29">
         <f>SUM(H29:H33)</f>
         <v>334555.21197341877</v>
       </c>
-      <c r="I35" s="32">
+      <c r="I35" s="29">
         <f>SUM(I28:I33)</f>
         <v>426521.29715512384</v>
       </c>
-      <c r="J35" s="33">
+      <c r="J35" s="30">
         <f>SUM(J27:J33)</f>
         <v>470894.29715512384</v>
       </c>
@@ -3045,9 +3106,9 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="79"/>
-      <c r="B36" s="79"/>
-      <c r="C36" s="79"/>
+      <c r="A36" s="70"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="70"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -3067,7 +3128,7 @@
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="79"/>
+      <c r="C37" s="70"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -3085,11 +3146,11 @@
       <c r="R37" s="2"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="92" t="s">
+      <c r="A38" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="92"/>
-      <c r="C38" s="80">
+      <c r="B38" s="154"/>
+      <c r="C38" s="71">
         <v>0.05</v>
       </c>
       <c r="D38" s="2"/>
@@ -3110,18 +3171,18 @@
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="81" t="s">
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="82"/>
-      <c r="K39" s="17"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="14"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
@@ -3132,38 +3193,38 @@
     </row>
     <row r="40" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="39">
+      <c r="B40" s="9"/>
+      <c r="C40" s="34">
         <v>2018</v>
       </c>
-      <c r="D40" s="16">
-        <f>C40+1</f>
+      <c r="D40" s="13">
+        <f t="shared" ref="D40:I40" si="11">C40+1</f>
         <v>2019</v>
       </c>
-      <c r="E40" s="16">
-        <f>D40+1</f>
+      <c r="E40" s="13">
+        <f t="shared" si="11"/>
         <v>2020</v>
       </c>
-      <c r="F40" s="16">
-        <f>E40+1</f>
+      <c r="F40" s="13">
+        <f t="shared" si="11"/>
         <v>2021</v>
       </c>
-      <c r="G40" s="16">
-        <f>F40+1</f>
+      <c r="G40" s="13">
+        <f t="shared" si="11"/>
         <v>2022</v>
       </c>
-      <c r="H40" s="16">
-        <f>G40+1</f>
+      <c r="H40" s="13">
+        <f t="shared" si="11"/>
         <v>2023</v>
       </c>
-      <c r="I40" s="16">
-        <f>H40+1</f>
+      <c r="I40" s="13">
+        <f t="shared" si="11"/>
         <v>2024</v>
       </c>
-      <c r="J40" s="61" t="s">
+      <c r="J40" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="K40" s="83" t="s">
+      <c r="K40" s="74" t="s">
         <v>17</v>
       </c>
       <c r="L40" s="2"/>
@@ -3176,42 +3237,42 @@
     </row>
     <row r="41" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="84">
+      <c r="C41" s="75">
         <f>D33-C33+E32-D32+F31-E31+G30-F30+H29-G29+I28-H28+J27-I27</f>
         <v>66587.791849184025</v>
       </c>
-      <c r="D41" s="85">
+      <c r="D41" s="76">
         <f>E33-D33+F32-E32+G31-F31+H30-G30+I29-H29+J28-I28</f>
         <v>49201.584568711958</v>
       </c>
-      <c r="E41" s="85">
+      <c r="E41" s="76">
         <f>F33-E33+G32-F32+H31-G31+I30-H30+J29-I29</f>
         <v>34048.809876885178</v>
       </c>
-      <c r="F41" s="85">
+      <c r="F41" s="76">
         <f>G33-F33+H32-G32+I31-H31+J30-I30</f>
         <v>20115.787458883497</v>
       </c>
-      <c r="G41" s="85">
+      <c r="G41" s="76">
         <f>H33-G33+I32-H32+J31-I31</f>
         <v>8533.8611983197479</v>
       </c>
-      <c r="H41" s="85">
+      <c r="H41" s="76">
         <f>I33-H33+J32-I32</f>
         <v>3236.4622031394247</v>
       </c>
-      <c r="I41" s="85">
+      <c r="I41" s="76">
         <f>J33-I33</f>
         <v>0</v>
       </c>
-      <c r="J41" s="36">
+      <c r="J41" s="33">
         <f>SUM(C41:I41)</f>
         <v>181724.29715512384</v>
       </c>
-      <c r="K41" s="86"/>
+      <c r="K41" s="77"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -3222,42 +3283,42 @@
     </row>
     <row r="42" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="68">
-        <f>C41/(1+$C$38)^(C40-0.5-($C$40-1))</f>
+      <c r="C42" s="60">
+        <f t="shared" ref="C42:I42" si="12">C41/(1+$C$38)^(C40-0.5-($C$40-1))</f>
         <v>64983.030923100428</v>
       </c>
-      <c r="D42" s="32">
-        <f>D41/(1+$C$38)^(D40-0.5-($C$40-1))</f>
+      <c r="D42" s="29">
+        <f t="shared" si="12"/>
         <v>45729.361875989925</v>
       </c>
-      <c r="E42" s="32">
-        <f>E41/(1+$C$38)^(E40-0.5-($C$40-1))</f>
+      <c r="E42" s="29">
+        <f t="shared" si="12"/>
         <v>30138.989607857573</v>
       </c>
-      <c r="F42" s="32">
-        <f>F41/(1+$C$38)^(F40-0.5-($C$40-1))</f>
+      <c r="F42" s="29">
+        <f t="shared" si="12"/>
         <v>16957.994556563299</v>
       </c>
-      <c r="G42" s="32">
-        <f>G41/(1+$C$38)^(G40-0.5-($C$40-1))</f>
+      <c r="G42" s="29">
+        <f t="shared" si="12"/>
         <v>6851.6272672171763</v>
       </c>
-      <c r="H42" s="32">
-        <f>H41/(1+$C$38)^(H40-0.5-($C$40-1))</f>
+      <c r="H42" s="29">
+        <f t="shared" si="12"/>
         <v>2474.7389548996434</v>
       </c>
-      <c r="I42" s="32">
-        <f>I41/(1+$C$38)^(I40-0.5-($C$40-1))</f>
+      <c r="I42" s="29">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="J42" s="31">
+      <c r="J42" s="28">
         <f>SUM(C42:I42)</f>
         <v>167135.74318562803</v>
       </c>
-      <c r="K42" s="87">
+      <c r="K42" s="78">
         <f>J42</f>
         <v>167135.74318562803</v>
       </c>
@@ -3270,9 +3331,9 @@
       <c r="R42" s="2"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="79"/>
-      <c r="B43" s="79"/>
-      <c r="C43" s="79"/>
+      <c r="A43" s="70"/>
+      <c r="B43" s="70"/>
+      <c r="C43" s="70"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
@@ -3290,9 +3351,9 @@
       <c r="R43" s="2"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="79"/>
-      <c r="B44" s="79"/>
-      <c r="C44" s="79"/>
+      <c r="A44" s="70"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="70"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -3310,22 +3371,22 @@
       <c r="R44" s="2"/>
     </row>
     <row r="45" spans="1:18" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="57" t="s">
+      <c r="A45" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D45" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="60" t="s">
+      <c r="E45" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F45" s="46" t="s">
+      <c r="F45" s="41" t="s">
         <v>12</v>
       </c>
       <c r="G45" s="2"/>
@@ -3342,213 +3403,213 @@
       <c r="R45" s="2"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="61"/>
-      <c r="B46" s="62"/>
+      <c r="A46" s="53"/>
+      <c r="B46" s="54"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="27"/>
+      <c r="D46" s="24"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="46"/>
+      <c r="F46" s="41"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="27">
+      <c r="A47" s="24">
         <f>Data!B9</f>
         <v>2010</v>
       </c>
-      <c r="B47" s="63">
-        <f>J26</f>
+      <c r="B47" s="55">
+        <f t="shared" ref="B47:B54" si="13">J26</f>
         <v>48701</v>
       </c>
-      <c r="C47" s="24">
-        <f>B26</f>
+      <c r="C47" s="21">
+        <f t="shared" ref="C47:C54" si="14">B26</f>
         <v>60124.691358024691</v>
       </c>
-      <c r="D47" s="64">
-        <f>J26/B26</f>
+      <c r="D47" s="56">
+        <f t="shared" ref="D47:D54" si="15">J26/B26</f>
         <v>0.81</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="27">
-        <f>A47+1</f>
+      <c r="A48" s="24">
+        <f t="shared" ref="A48:A54" si="16">A47+1</f>
         <v>2011</v>
       </c>
-      <c r="B48" s="63">
-        <f>J27</f>
+      <c r="B48" s="55">
+        <f t="shared" si="13"/>
         <v>44373</v>
       </c>
-      <c r="C48" s="24">
-        <f>B27</f>
+      <c r="C48" s="21">
+        <f t="shared" si="14"/>
         <v>65235.290123456791</v>
       </c>
-      <c r="D48" s="64">
-        <f>J27/B27</f>
+      <c r="D48" s="56">
+        <f t="shared" si="15"/>
         <v>0.68019932027626118</v>
       </c>
       <c r="E48" s="2"/>
-      <c r="F48" s="24">
+      <c r="F48" s="21">
         <f>J27-I27</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="27">
-        <f>A48+1</f>
+      <c r="A49" s="24">
+        <f t="shared" si="16"/>
         <v>2012</v>
       </c>
-      <c r="B49" s="63">
-        <f>J28</f>
+      <c r="B49" s="55">
+        <f t="shared" si="13"/>
         <v>75282.814285232045</v>
       </c>
-      <c r="C49" s="24">
-        <f>B28</f>
+      <c r="C49" s="21">
+        <f t="shared" si="14"/>
         <v>75281.524802469125</v>
       </c>
-      <c r="D49" s="64">
-        <f>J28/B28</f>
+      <c r="D49" s="56">
+        <f t="shared" si="15"/>
         <v>1.0000171288077162</v>
       </c>
       <c r="E49" s="2"/>
-      <c r="F49" s="24">
+      <c r="F49" s="21">
         <f>J28-H28</f>
         <v>3575.8142852320452</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="27">
-        <f>A49+1</f>
+      <c r="A50" s="24">
+        <f t="shared" si="16"/>
         <v>2013</v>
       </c>
-      <c r="B50" s="63">
-        <f>J29</f>
+      <c r="B50" s="55">
+        <f t="shared" si="13"/>
         <v>82006.620952928744</v>
       </c>
-      <c r="C50" s="24">
-        <f>B29</f>
+      <c r="C50" s="21">
+        <f t="shared" si="14"/>
         <v>78970.319517790107</v>
       </c>
-      <c r="D50" s="64">
-        <f>J29/B29</f>
+      <c r="D50" s="56">
+        <f t="shared" si="15"/>
         <v>1.0384486406244644</v>
       </c>
       <c r="E50" s="2"/>
-      <c r="F50" s="67">
+      <c r="F50" s="59">
         <f>J29-G29</f>
         <v>10316.620952928744</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="27">
-        <f>A50+1</f>
+      <c r="A51" s="24">
+        <f t="shared" si="16"/>
         <v>2014</v>
       </c>
-      <c r="B51" s="63">
-        <f>J30</f>
+      <c r="B51" s="55">
+        <f t="shared" si="13"/>
         <v>69613.186288457</v>
       </c>
-      <c r="C51" s="24">
-        <f>B30</f>
+      <c r="C51" s="21">
+        <f t="shared" si="14"/>
         <v>80154.874310556945</v>
       </c>
-      <c r="D51" s="64">
-        <f>J30/B30</f>
+      <c r="D51" s="56">
+        <f t="shared" si="15"/>
         <v>0.86848350630235427</v>
       </c>
       <c r="E51" s="2"/>
-      <c r="F51" s="67">
+      <c r="F51" s="59">
         <f>J30-F30</f>
         <v>20809.186288457</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="27">
-        <f>A51+1</f>
+      <c r="A52" s="24">
+        <f t="shared" si="16"/>
         <v>2015</v>
       </c>
-      <c r="B52" s="63">
-        <f>J31</f>
+      <c r="B52" s="55">
+        <f t="shared" si="13"/>
         <v>64144.07794562848</v>
       </c>
-      <c r="C52" s="24">
-        <f>B31</f>
+      <c r="C52" s="21">
+        <f t="shared" si="14"/>
         <v>76948.679338134665</v>
       </c>
-      <c r="D52" s="64">
-        <f>J31/B31</f>
+      <c r="D52" s="56">
+        <f t="shared" si="15"/>
         <v>0.83359556651727473</v>
       </c>
       <c r="E52" s="2"/>
-      <c r="F52" s="67">
+      <c r="F52" s="59">
         <f>J31-E31</f>
         <v>32412.07794562848</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="27">
-        <f>A52+1</f>
+      <c r="A53" s="24">
+        <f t="shared" si="16"/>
         <v>2016</v>
       </c>
-      <c r="B53" s="63">
-        <f>J32</f>
+      <c r="B53" s="55">
+        <f t="shared" si="13"/>
         <v>67336.276297904711</v>
       </c>
-      <c r="C53" s="24">
-        <f>B32</f>
+      <c r="C53" s="21">
+        <f t="shared" si="14"/>
         <v>75409.705751371977</v>
       </c>
-      <c r="D53" s="64">
-        <f>J32/B32</f>
+      <c r="D53" s="56">
+        <f t="shared" si="15"/>
         <v>0.89293912006386023</v>
       </c>
       <c r="E53" s="2"/>
-      <c r="F53" s="67">
+      <c r="F53" s="59">
         <f>J32-D32</f>
         <v>48704.276297904711</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="27">
-        <f>A53+1</f>
+      <c r="A54" s="24">
+        <f t="shared" si="16"/>
         <v>2017</v>
       </c>
-      <c r="B54" s="68">
-        <f>J33</f>
+      <c r="B54" s="60">
+        <f t="shared" si="13"/>
         <v>68138.321384972834</v>
       </c>
-      <c r="C54" s="69">
-        <f>B33</f>
+      <c r="C54" s="61">
+        <f t="shared" si="14"/>
         <v>77294.948395156272</v>
       </c>
-      <c r="D54" s="70"/>
-      <c r="E54" s="71">
+      <c r="D54" s="62"/>
+      <c r="E54" s="63">
         <f>D55*B33-C33</f>
         <v>65906.321384972834</v>
       </c>
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
-      <c r="B55" s="73" t="s">
+      <c r="A55" s="27"/>
+      <c r="B55" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="C55" s="73"/>
-      <c r="D55" s="74">
+      <c r="C55" s="153"/>
+      <c r="D55" s="65">
         <f>SUM(J26:J32)/SUM(B26:B32)</f>
         <v>0.88153654022288941</v>
       </c>
-      <c r="E55" s="75" t="str">
+      <c r="E55" s="66" t="str">
         <f>" for "&amp;A26&amp;" to "&amp;A32</f>
         <v xml:space="preserve"> for 2010 to 2016</v>
       </c>
-      <c r="F55" s="76"/>
+      <c r="F55" s="67"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="77" t="s">
+      <c r="A56" s="68" t="s">
         <v>12</v>
       </c>
       <c r="B56" s="2"/>
-      <c r="C56" s="67">
+      <c r="C56" s="59">
         <f>SUM(F48:F54)</f>
         <v>115817.97577015098</v>
       </c>
@@ -3567,15 +3628,16 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241DE72D-CA3B-4A7C-8C20-F0F181E3C5E6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3587,1058 +3649,1058 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="79" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="159" t="s">
+      <c r="A4" s="140" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="94"/>
-      <c r="B5" s="95"/>
-      <c r="C5" s="96" t="s">
+      <c r="A5" s="80"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="98"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="156"/>
+      <c r="H5" s="156"/>
+      <c r="I5" s="156"/>
+      <c r="J5" s="157"/>
     </row>
     <row r="6" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="144" t="s">
+      <c r="A6" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="149" t="s">
+      <c r="B6" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="144">
+      <c r="C6" s="127">
         <v>0</v>
       </c>
-      <c r="D6" s="145">
-        <f>C6+12</f>
+      <c r="D6" s="128">
+        <f t="shared" ref="D6:J6" si="0">C6+12</f>
         <v>12</v>
       </c>
-      <c r="E6" s="145">
-        <f>D6+12</f>
+      <c r="E6" s="128">
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="F6" s="145">
-        <f>E6+12</f>
+      <c r="F6" s="128">
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="G6" s="145">
-        <f>F6+12</f>
+      <c r="G6" s="128">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="H6" s="145">
-        <f>G6+12</f>
+      <c r="H6" s="128">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="I6" s="145">
-        <f>H6+12</f>
+      <c r="I6" s="128">
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="J6" s="150">
-        <f>I6+12</f>
+      <c r="J6" s="131">
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="151"/>
-      <c r="B7" s="152"/>
-      <c r="C7" s="151"/>
-      <c r="D7" s="153"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="153"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="154"/>
+      <c r="A7" s="132"/>
+      <c r="B7" s="133"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="134"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="134"/>
+      <c r="G7" s="134"/>
+      <c r="H7" s="134"/>
+      <c r="I7" s="134"/>
+      <c r="J7" s="135"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="106">
+      <c r="A8" s="89">
         <f>Calculations!A26</f>
         <v>2010</v>
       </c>
-      <c r="B8" s="107">
+      <c r="B8" s="90">
         <f>Calculations!B26</f>
         <v>60124.691358024691</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="21">
         <f>Calculations!C26</f>
         <v>3330.86</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <f>Calculations!D26</f>
         <v>12811</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="21">
         <f>Calculations!E26</f>
         <v>20370</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="21">
         <f>Calculations!F26</f>
         <v>26656</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="21">
         <f>Calculations!G26</f>
         <v>37667</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="21">
         <f>Calculations!H26</f>
         <v>44414</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="21">
         <f>Calculations!I26</f>
         <v>48701</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="22">
         <f>Calculations!J26</f>
         <v>48701</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="106">
+      <c r="A9" s="89">
         <f>Calculations!A27</f>
         <v>2011</v>
       </c>
-      <c r="B9" s="107">
+      <c r="B9" s="90">
         <f>Calculations!B27</f>
         <v>65235.290123456791</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="21">
         <f>Calculations!C27</f>
         <v>1447.6499999999999</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <f>Calculations!D27</f>
         <v>9651</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="21">
         <f>Calculations!E27</f>
         <v>16995</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="21">
         <f>Calculations!F27</f>
         <v>30354</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="21">
         <f>Calculations!G27</f>
         <v>40594</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="21">
         <f>Calculations!H27</f>
         <v>44231</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="21">
         <f>Calculations!I27</f>
         <v>44373</v>
       </c>
-      <c r="J9" s="65">
+      <c r="J9" s="57">
         <f>Calculations!J27</f>
         <v>44373</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="106">
+      <c r="A10" s="89">
         <f>Calculations!A28</f>
         <v>2012</v>
       </c>
-      <c r="B10" s="107">
+      <c r="B10" s="90">
         <f>Calculations!B28</f>
         <v>75281.524802469125</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="21">
         <f>Calculations!C28</f>
         <v>1529.55</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <f>Calculations!D28</f>
         <v>16995</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <f>Calculations!E28</f>
         <v>40180</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="21">
         <f>Calculations!F28</f>
         <v>58866</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="21">
         <f>Calculations!G28</f>
         <v>71707</v>
       </c>
-      <c r="H10" s="24">
+      <c r="H10" s="21">
         <f>Calculations!H28</f>
         <v>71707</v>
       </c>
-      <c r="I10" s="66">
+      <c r="I10" s="58">
         <f>Calculations!I28</f>
         <v>75282.814285232045</v>
       </c>
-      <c r="J10" s="65">
+      <c r="J10" s="57">
         <f>Calculations!J28</f>
         <v>75282.814285232045</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="106">
+      <c r="A11" s="89">
         <f>Calculations!A29</f>
         <v>2013</v>
       </c>
-      <c r="B11" s="107">
+      <c r="B11" s="90">
         <f>Calculations!B29</f>
         <v>78970.319517790107</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="21">
         <f>Calculations!C29</f>
         <v>5161.32</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <f>Calculations!D29</f>
         <v>28674</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="21">
         <f>Calculations!E29</f>
         <v>47432</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="21">
         <f>Calculations!F29</f>
         <v>70340</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="21">
         <f>Calculations!G29</f>
         <v>71690</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="58">
         <f>Calculations!H29</f>
         <v>78111.436514471628</v>
       </c>
-      <c r="I11" s="66">
+      <c r="I11" s="58">
         <f>Calculations!I29</f>
         <v>82006.620952928744</v>
       </c>
-      <c r="J11" s="65">
+      <c r="J11" s="57">
         <f>Calculations!J29</f>
         <v>82006.620952928744</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="106">
+      <c r="A12" s="89">
         <f>Calculations!A30</f>
         <v>2014</v>
       </c>
-      <c r="B12" s="107">
+      <c r="B12" s="90">
         <f>Calculations!B30</f>
         <v>80154.874310556945</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="21">
         <f>Calculations!C30</f>
         <v>6225.18</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="21">
         <f>Calculations!D30</f>
         <v>27066</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="21">
         <f>Calculations!E30</f>
         <v>46783</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="21">
         <f>Calculations!F30</f>
         <v>48804</v>
       </c>
-      <c r="G12" s="66">
+      <c r="G12" s="58">
         <f>Calculations!G30</f>
         <v>60855.687833840107</v>
       </c>
-      <c r="H12" s="66">
+      <c r="H12" s="58">
         <f>Calculations!H30</f>
         <v>66306.670341435412</v>
       </c>
-      <c r="I12" s="66">
+      <c r="I12" s="58">
         <f>Calculations!I30</f>
         <v>69613.186288457</v>
       </c>
-      <c r="J12" s="65">
+      <c r="J12" s="57">
         <f>Calculations!J30</f>
         <v>69613.186288457</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="106">
+      <c r="A13" s="89">
         <f>Calculations!A31</f>
         <v>2015</v>
       </c>
-      <c r="B13" s="107">
+      <c r="B13" s="90">
         <f>Calculations!B31</f>
         <v>76948.679338134665</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="21">
         <f>Calculations!C31</f>
         <v>4325</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="21">
         <f>Calculations!D31</f>
         <v>19477</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="21">
         <f>Calculations!E31</f>
         <v>31732</v>
       </c>
-      <c r="F13" s="66">
+      <c r="F13" s="58">
         <f>Calculations!F31</f>
         <v>44969.749942009737</v>
       </c>
-      <c r="G13" s="66">
+      <c r="G13" s="58">
         <f>Calculations!G31</f>
         <v>56074.605860929303</v>
       </c>
-      <c r="H13" s="66">
+      <c r="H13" s="58">
         <f>Calculations!H31</f>
         <v>61097.335971265144</v>
       </c>
-      <c r="I13" s="66">
+      <c r="I13" s="58">
         <f>Calculations!I31</f>
         <v>64144.07794562848</v>
       </c>
-      <c r="J13" s="65">
+      <c r="J13" s="57">
         <f>Calculations!J31</f>
         <v>64144.07794562848</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="106">
+      <c r="A14" s="89">
         <f>Calculations!A32</f>
         <v>2016</v>
       </c>
-      <c r="B14" s="107">
+      <c r="B14" s="90">
         <f>Calculations!B32</f>
         <v>75409.705751371977</v>
       </c>
-      <c r="C14" s="110">
+      <c r="C14" s="93">
         <f>Calculations!C32</f>
         <v>931.6</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="21">
         <f>Calculations!D32</f>
         <v>18632</v>
       </c>
-      <c r="E14" s="66">
+      <c r="E14" s="58">
         <f>Calculations!E32</f>
         <v>33311.176774515203</v>
       </c>
-      <c r="F14" s="66">
+      <c r="F14" s="58">
         <f>Calculations!F32</f>
         <v>47207.717440565713</v>
       </c>
-      <c r="G14" s="66">
+      <c r="G14" s="58">
         <f>Calculations!G32</f>
         <v>58865.218340939187</v>
       </c>
-      <c r="H14" s="66">
+      <c r="H14" s="58">
         <f>Calculations!H32</f>
         <v>64137.9099644132</v>
       </c>
-      <c r="I14" s="66">
+      <c r="I14" s="58">
         <f>Calculations!I32</f>
         <v>67336.276297904711</v>
       </c>
-      <c r="J14" s="65">
+      <c r="J14" s="57">
         <f>Calculations!J32</f>
         <v>67336.276297904711</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="108">
+      <c r="A15" s="91">
         <f>Calculations!A33</f>
         <v>2017</v>
       </c>
-      <c r="B15" s="109">
+      <c r="B15" s="92">
         <f>Calculations!B33</f>
         <v>77294.948395156272</v>
       </c>
-      <c r="C15" s="111">
+      <c r="C15" s="94">
         <f>Calculations!C33</f>
         <v>2232</v>
       </c>
-      <c r="D15" s="112">
+      <c r="D15" s="95">
         <f>Calculations!D33</f>
         <v>18853.926499115285</v>
       </c>
-      <c r="E15" s="112">
+      <c r="E15" s="95">
         <f>Calculations!E33</f>
         <v>33707.947536804735</v>
       </c>
-      <c r="F15" s="112">
+      <c r="F15" s="95">
         <f>Calculations!F33</f>
         <v>47770.010455959025</v>
       </c>
-      <c r="G15" s="112">
+      <c r="G15" s="95">
         <f>Calculations!G33</f>
         <v>59566.364317005166</v>
       </c>
-      <c r="H15" s="112">
+      <c r="H15" s="95">
         <f>Calculations!H33</f>
         <v>64901.85918183341</v>
       </c>
-      <c r="I15" s="112">
+      <c r="I15" s="95">
         <f>Calculations!I33</f>
         <v>68138.321384972834</v>
       </c>
-      <c r="J15" s="113">
+      <c r="J15" s="96">
         <f>Calculations!J33</f>
         <v>68138.321384972834</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="159" t="s">
+      <c r="A18" s="140" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="139"/>
-      <c r="B19" s="146"/>
-      <c r="C19" s="147" t="s">
+      <c r="A19" s="122"/>
+      <c r="B19" s="129"/>
+      <c r="C19" s="158" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="147"/>
-      <c r="E19" s="147"/>
-      <c r="F19" s="147"/>
-      <c r="G19" s="147"/>
-      <c r="H19" s="147"/>
-      <c r="I19" s="147"/>
-      <c r="J19" s="148"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
+      <c r="H19" s="158"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="159"/>
     </row>
     <row r="20" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="143" t="s">
+      <c r="A20" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="149" t="s">
+      <c r="B20" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="145">
+      <c r="C20" s="128">
         <v>0</v>
       </c>
-      <c r="D20" s="145">
+      <c r="D20" s="128">
         <v>12</v>
       </c>
-      <c r="E20" s="145">
-        <f>D20+12</f>
+      <c r="E20" s="128">
+        <f t="shared" ref="E20:J20" si="1">D20+12</f>
         <v>24</v>
       </c>
-      <c r="F20" s="145">
-        <f>E20+12</f>
+      <c r="F20" s="128">
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="G20" s="145">
-        <f>F20+12</f>
+      <c r="G20" s="128">
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="H20" s="145">
-        <f>G20+12</f>
+      <c r="H20" s="128">
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="I20" s="145">
-        <f>H20+12</f>
+      <c r="I20" s="128">
+        <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="J20" s="150">
-        <f>I20+12</f>
+      <c r="J20" s="131">
+        <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="100"/>
-      <c r="I21" s="100"/>
-      <c r="J21" s="101"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="83"/>
+      <c r="H21" s="83"/>
+      <c r="I21" s="83"/>
+      <c r="J21" s="84"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="42">
+      <c r="A22" s="37">
         <f>Calculations!A6</f>
         <v>2010</v>
       </c>
-      <c r="B22" s="117">
+      <c r="B22" s="100">
         <f>Calculations!B6</f>
         <v>60124.691358024691</v>
       </c>
-      <c r="C22" s="118"/>
-      <c r="D22" s="114">
+      <c r="C22" s="101"/>
+      <c r="D22" s="97">
         <f>Calculations!D6</f>
         <v>3.8461538461538458</v>
       </c>
-      <c r="E22" s="114">
+      <c r="E22" s="97">
         <f>Calculations!E6</f>
         <v>1.5900398095386776</v>
       </c>
-      <c r="F22" s="114">
+      <c r="F22" s="97">
         <f>Calculations!F6</f>
         <v>1.3085910652920962</v>
       </c>
-      <c r="G22" s="114">
+      <c r="G22" s="97">
         <f>Calculations!G6</f>
         <v>1.413077731092437</v>
       </c>
-      <c r="H22" s="114">
+      <c r="H22" s="97">
         <f>Calculations!H6</f>
         <v>1.1791223086521359</v>
       </c>
-      <c r="I22" s="114">
+      <c r="I22" s="97">
         <f>Calculations!I6</f>
         <v>1.096523618678795</v>
       </c>
-      <c r="J22" s="119">
+      <c r="J22" s="102">
         <f>Calculations!J6</f>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="42">
+      <c r="A23" s="37">
         <f>Calculations!A7</f>
         <v>2011</v>
       </c>
-      <c r="B23" s="117">
+      <c r="B23" s="100">
         <f>Calculations!B7</f>
         <v>65235.290123456791</v>
       </c>
-      <c r="C23" s="117"/>
-      <c r="D23" s="114">
+      <c r="C23" s="100"/>
+      <c r="D23" s="97">
         <f>Calculations!D7</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="E23" s="114">
+      <c r="E23" s="97">
         <f>Calculations!E7</f>
         <v>1.7609574137395088</v>
       </c>
-      <c r="F23" s="114">
+      <c r="F23" s="97">
         <f>Calculations!F7</f>
         <v>1.7860547219770522</v>
       </c>
-      <c r="G23" s="114">
+      <c r="G23" s="97">
         <f>Calculations!G7</f>
         <v>1.3373525729722606</v>
       </c>
-      <c r="H23" s="114">
+      <c r="H23" s="97">
         <f>Calculations!H7</f>
         <v>1.0895945213578362</v>
       </c>
-      <c r="I23" s="114">
+      <c r="I23" s="97">
         <f>Calculations!I7</f>
         <v>1.0032104180326016</v>
       </c>
-      <c r="J23" s="120"/>
+      <c r="J23" s="103"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="42">
+      <c r="A24" s="37">
         <f>Calculations!A8</f>
         <v>2012</v>
       </c>
-      <c r="B24" s="117">
+      <c r="B24" s="100">
         <f>Calculations!B8</f>
         <v>75281.524802469125</v>
       </c>
-      <c r="C24" s="117"/>
-      <c r="D24" s="114">
+      <c r="C24" s="100"/>
+      <c r="D24" s="97">
         <f>Calculations!D8</f>
         <v>11.111111111111111</v>
       </c>
-      <c r="E24" s="114">
+      <c r="E24" s="97">
         <f>Calculations!E8</f>
         <v>2.3642247719917622</v>
       </c>
-      <c r="F24" s="114">
+      <c r="F24" s="97">
         <f>Calculations!F8</f>
         <v>1.4650572424091588</v>
       </c>
-      <c r="G24" s="114">
+      <c r="G24" s="97">
         <f>Calculations!G8</f>
         <v>1.2181395032786329</v>
       </c>
-      <c r="H24" s="114">
+      <c r="H24" s="97">
         <f>Calculations!H8</f>
         <v>1</v>
       </c>
-      <c r="I24" s="115"/>
-      <c r="J24" s="120"/>
+      <c r="I24" s="98"/>
+      <c r="J24" s="103"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="42">
+      <c r="A25" s="37">
         <f>Calculations!A9</f>
         <v>2013</v>
       </c>
-      <c r="B25" s="117">
+      <c r="B25" s="100">
         <f>Calculations!B9</f>
         <v>78970.319517790107</v>
       </c>
-      <c r="C25" s="117"/>
-      <c r="D25" s="114">
+      <c r="C25" s="100"/>
+      <c r="D25" s="97">
         <f>Calculations!D9</f>
         <v>5.5555555555555562</v>
       </c>
-      <c r="E25" s="114">
+      <c r="E25" s="97">
         <f>Calculations!E9</f>
         <v>1.6541814884564414</v>
       </c>
-      <c r="F25" s="114">
+      <c r="F25" s="97">
         <f>Calculations!F9</f>
         <v>1.4829650868611908</v>
       </c>
-      <c r="G25" s="114">
+      <c r="G25" s="97">
         <f>Calculations!G9</f>
         <v>1.0191924936025021</v>
       </c>
-      <c r="H25" s="115"/>
-      <c r="I25" s="115"/>
-      <c r="J25" s="120"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="103"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="42">
+      <c r="A26" s="37">
         <f>Calculations!A10</f>
         <v>2014</v>
       </c>
-      <c r="B26" s="117">
+      <c r="B26" s="100">
         <f>Calculations!B10</f>
         <v>80154.874310556945</v>
       </c>
-      <c r="C26" s="117"/>
-      <c r="D26" s="114">
+      <c r="C26" s="100"/>
+      <c r="D26" s="97">
         <f>Calculations!D10</f>
         <v>4.3478260869565215</v>
       </c>
-      <c r="E26" s="114">
+      <c r="E26" s="97">
         <f>Calculations!E10</f>
         <v>1.7284785339540383</v>
       </c>
-      <c r="F26" s="114">
+      <c r="F26" s="97">
         <f>Calculations!F10</f>
         <v>1.0431994527926811</v>
       </c>
-      <c r="G26" s="115"/>
-      <c r="H26" s="115"/>
-      <c r="I26" s="115"/>
-      <c r="J26" s="120"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="98"/>
+      <c r="I26" s="98"/>
+      <c r="J26" s="103"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="42">
+      <c r="A27" s="37">
         <f>Calculations!A11</f>
         <v>2015</v>
       </c>
-      <c r="B27" s="117">
+      <c r="B27" s="100">
         <f>Calculations!B11</f>
         <v>76948.679338134665</v>
       </c>
-      <c r="C27" s="117"/>
-      <c r="D27" s="114">
+      <c r="C27" s="100"/>
+      <c r="D27" s="97">
         <f>Calculations!D11</f>
         <v>4.5033526011560694</v>
       </c>
-      <c r="E27" s="114">
+      <c r="E27" s="97">
         <f>Calculations!E11</f>
         <v>1.6292036761308211</v>
       </c>
-      <c r="F27" s="115"/>
-      <c r="G27" s="115"/>
-      <c r="H27" s="115"/>
-      <c r="I27" s="115"/>
-      <c r="J27" s="120"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="103"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="42">
+      <c r="A28" s="37">
         <f>Calculations!A12</f>
         <v>2016</v>
       </c>
-      <c r="B28" s="117">
+      <c r="B28" s="100">
         <f>Calculations!B12</f>
         <v>75409.705751371977</v>
       </c>
-      <c r="C28" s="117"/>
-      <c r="D28" s="114">
+      <c r="C28" s="100"/>
+      <c r="D28" s="97">
         <f>Calculations!D12</f>
         <v>20</v>
       </c>
-      <c r="E28" s="115"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="115"/>
-      <c r="H28" s="115"/>
-      <c r="I28" s="115"/>
-      <c r="J28" s="120"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="98"/>
+      <c r="H28" s="98"/>
+      <c r="I28" s="98"/>
+      <c r="J28" s="103"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="42">
+      <c r="A29" s="37">
         <f>Calculations!A13</f>
         <v>2017</v>
       </c>
-      <c r="B29" s="117">
+      <c r="B29" s="100">
         <f>Calculations!B13</f>
         <v>77294.948395156272</v>
       </c>
-      <c r="C29" s="117"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
-      <c r="G29" s="121"/>
-      <c r="H29" s="121"/>
-      <c r="I29" s="121"/>
-      <c r="J29" s="122"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="104"/>
+      <c r="E29" s="104"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="104"/>
+      <c r="H29" s="104"/>
+      <c r="I29" s="104"/>
+      <c r="J29" s="105"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="117"/>
-      <c r="C30" s="117"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="123"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="100"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="106"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="127" t="s">
+      <c r="A31" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="116"/>
-      <c r="C31" s="126"/>
-      <c r="D31" s="124"/>
-      <c r="E31" s="124">
-        <f>AVERAGE(E22:E28)</f>
+      <c r="B31" s="99"/>
+      <c r="C31" s="109"/>
+      <c r="D31" s="107"/>
+      <c r="E31" s="107">
+        <f t="shared" ref="E31:J31" si="2">AVERAGE(E22:E28)</f>
         <v>1.7878476156352086</v>
       </c>
-      <c r="F31" s="124">
-        <f>AVERAGE(F22:F28)</f>
+      <c r="F31" s="107">
+        <f t="shared" si="2"/>
         <v>1.4171735138664356</v>
       </c>
-      <c r="G31" s="124">
-        <f>AVERAGE(G22:G28)</f>
+      <c r="G31" s="107">
+        <f t="shared" si="2"/>
         <v>1.2469405752364582</v>
       </c>
-      <c r="H31" s="124">
-        <f>AVERAGE(H22:H28)</f>
+      <c r="H31" s="107">
+        <f t="shared" si="2"/>
         <v>1.0895722766699907</v>
       </c>
-      <c r="I31" s="124">
-        <f>AVERAGE(I22:I28)</f>
+      <c r="I31" s="107">
+        <f t="shared" si="2"/>
         <v>1.0498670183556982</v>
       </c>
-      <c r="J31" s="125">
-        <f>AVERAGE(J22:J28)</f>
+      <c r="J31" s="108">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="159" t="s">
+      <c r="A34" s="140" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="140"/>
-      <c r="B35" s="140"/>
-      <c r="C35" s="141" t="s">
+      <c r="A35" s="123"/>
+      <c r="B35" s="123"/>
+      <c r="C35" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="141"/>
-      <c r="E35" s="141"/>
-      <c r="F35" s="141"/>
-      <c r="G35" s="141"/>
-      <c r="H35" s="141"/>
-      <c r="I35" s="142"/>
-      <c r="J35" s="130"/>
+      <c r="D35" s="124"/>
+      <c r="E35" s="124"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="124"/>
+      <c r="H35" s="124"/>
+      <c r="I35" s="125"/>
+      <c r="J35" s="113"/>
     </row>
     <row r="36" spans="1:10" ht="39" x14ac:dyDescent="0.25">
-      <c r="A36" s="143"/>
-      <c r="B36" s="144">
+      <c r="A36" s="126"/>
+      <c r="B36" s="127">
         <v>2018</v>
       </c>
-      <c r="C36" s="145">
-        <f>B36+1</f>
+      <c r="C36" s="128">
+        <f t="shared" ref="C36:H36" si="3">B36+1</f>
         <v>2019</v>
       </c>
-      <c r="D36" s="145">
-        <f>C36+1</f>
+      <c r="D36" s="128">
+        <f t="shared" si="3"/>
         <v>2020</v>
       </c>
-      <c r="E36" s="145">
-        <f>D36+1</f>
+      <c r="E36" s="128">
+        <f t="shared" si="3"/>
         <v>2021</v>
       </c>
-      <c r="F36" s="145">
-        <f>E36+1</f>
+      <c r="F36" s="128">
+        <f t="shared" si="3"/>
         <v>2022</v>
       </c>
-      <c r="G36" s="145">
-        <f>F36+1</f>
+      <c r="G36" s="128">
+        <f t="shared" si="3"/>
         <v>2023</v>
       </c>
-      <c r="H36" s="145">
-        <f>G36+1</f>
+      <c r="H36" s="128">
+        <f t="shared" si="3"/>
         <v>2024</v>
       </c>
-      <c r="I36" s="144" t="s">
+      <c r="I36" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="J36" s="129" t="s">
+      <c r="J36" s="112" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="131">
+      <c r="B37" s="114">
         <f>Calculations!C41</f>
         <v>66587.791849184025</v>
       </c>
-      <c r="C37" s="132">
+      <c r="C37" s="115">
         <f>Calculations!D41</f>
         <v>49201.584568711958</v>
       </c>
-      <c r="D37" s="132">
+      <c r="D37" s="115">
         <f>Calculations!E41</f>
         <v>34048.809876885178</v>
       </c>
-      <c r="E37" s="132">
+      <c r="E37" s="115">
         <f>Calculations!F41</f>
         <v>20115.787458883497</v>
       </c>
-      <c r="F37" s="132">
+      <c r="F37" s="115">
         <f>Calculations!G41</f>
         <v>8533.8611983197479</v>
       </c>
-      <c r="G37" s="132">
+      <c r="G37" s="115">
         <f>Calculations!H41</f>
         <v>3236.4622031394247</v>
       </c>
-      <c r="H37" s="132">
+      <c r="H37" s="115">
         <f>Calculations!I41</f>
         <v>0</v>
       </c>
-      <c r="I37" s="135">
+      <c r="I37" s="118">
         <f>Calculations!J41</f>
         <v>181724.29715512384</v>
       </c>
-      <c r="J37" s="103"/>
+      <c r="J37" s="86"/>
     </row>
     <row r="38" spans="1:10" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="111">
+      <c r="B38" s="94">
         <f>Calculations!C42</f>
         <v>64983.030923100428</v>
       </c>
-      <c r="C38" s="133">
+      <c r="C38" s="116">
         <f>Calculations!D42</f>
         <v>45729.361875989925</v>
       </c>
-      <c r="D38" s="133">
+      <c r="D38" s="116">
         <f>Calculations!E42</f>
         <v>30138.989607857573</v>
       </c>
-      <c r="E38" s="133">
+      <c r="E38" s="116">
         <f>Calculations!F42</f>
         <v>16957.994556563299</v>
       </c>
-      <c r="F38" s="133">
+      <c r="F38" s="116">
         <f>Calculations!G42</f>
         <v>6851.6272672171763</v>
       </c>
-      <c r="G38" s="133">
+      <c r="G38" s="116">
         <f>Calculations!H42</f>
         <v>2474.7389548996434</v>
       </c>
-      <c r="H38" s="133">
+      <c r="H38" s="116">
         <f>Calculations!I42</f>
         <v>0</v>
       </c>
-      <c r="I38" s="128">
+      <c r="I38" s="111">
         <f>Calculations!J42</f>
         <v>167135.74318562803</v>
       </c>
-      <c r="J38" s="134">
+      <c r="J38" s="117">
         <f>Calculations!K42</f>
         <v>167135.74318562803</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="159" t="s">
+      <c r="A40" s="140" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="136" t="s">
+      <c r="A41" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="137" t="s">
+      <c r="B41" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="138" t="s">
+      <c r="C41" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="D41" s="139" t="s">
+      <c r="D41" s="122" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="42">
+      <c r="A42" s="37">
         <f>Calculations!A47</f>
         <v>2010</v>
       </c>
-      <c r="B42" s="156">
+      <c r="B42" s="137">
         <f>Calculations!B47</f>
         <v>48701</v>
       </c>
-      <c r="C42" s="157">
+      <c r="C42" s="138">
         <f>Calculations!C47</f>
         <v>60124.691358024691</v>
       </c>
-      <c r="D42" s="155">
+      <c r="D42" s="136">
         <f>Calculations!D47</f>
         <v>0.81</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="42">
+      <c r="A43" s="37">
         <f>Calculations!A48</f>
         <v>2011</v>
       </c>
-      <c r="B43" s="102">
+      <c r="B43" s="85">
         <f>Calculations!B48</f>
         <v>44373</v>
       </c>
-      <c r="C43" s="103">
+      <c r="C43" s="86">
         <f>Calculations!C48</f>
         <v>65235.290123456791</v>
       </c>
-      <c r="D43" s="155">
+      <c r="D43" s="136">
         <f>Calculations!D48</f>
         <v>0.68019932027626118</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="42">
+      <c r="A44" s="37">
         <f>Calculations!A49</f>
         <v>2012</v>
       </c>
-      <c r="B44" s="102">
+      <c r="B44" s="85">
         <f>Calculations!B49</f>
         <v>75282.814285232045</v>
       </c>
-      <c r="C44" s="103">
+      <c r="C44" s="86">
         <f>Calculations!C49</f>
         <v>75281.524802469125</v>
       </c>
-      <c r="D44" s="155">
+      <c r="D44" s="136">
         <f>Calculations!D49</f>
         <v>1.0000171288077162</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="42">
+      <c r="A45" s="37">
         <f>Calculations!A50</f>
         <v>2013</v>
       </c>
-      <c r="B45" s="102">
+      <c r="B45" s="85">
         <f>Calculations!B50</f>
         <v>82006.620952928744</v>
       </c>
-      <c r="C45" s="103">
+      <c r="C45" s="86">
         <f>Calculations!C50</f>
         <v>78970.319517790107</v>
       </c>
-      <c r="D45" s="155">
+      <c r="D45" s="136">
         <f>Calculations!D50</f>
         <v>1.0384486406244644</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="42">
+      <c r="A46" s="37">
         <f>Calculations!A51</f>
         <v>2014</v>
       </c>
-      <c r="B46" s="102">
+      <c r="B46" s="85">
         <f>Calculations!B51</f>
         <v>69613.186288457</v>
       </c>
-      <c r="C46" s="103">
+      <c r="C46" s="86">
         <f>Calculations!C51</f>
         <v>80154.874310556945</v>
       </c>
-      <c r="D46" s="155">
+      <c r="D46" s="136">
         <f>Calculations!D51</f>
         <v>0.86848350630235427</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="42">
+      <c r="A47" s="37">
         <f>Calculations!A52</f>
         <v>2015</v>
       </c>
-      <c r="B47" s="102">
+      <c r="B47" s="85">
         <f>Calculations!B52</f>
         <v>64144.07794562848</v>
       </c>
-      <c r="C47" s="103">
+      <c r="C47" s="86">
         <f>Calculations!C52</f>
         <v>76948.679338134665</v>
       </c>
-      <c r="D47" s="155">
+      <c r="D47" s="136">
         <f>Calculations!D52</f>
         <v>0.83359556651727473</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="42">
+      <c r="A48" s="37">
         <f>Calculations!A53</f>
         <v>2016</v>
       </c>
-      <c r="B48" s="102">
+      <c r="B48" s="85">
         <f>Calculations!B53</f>
         <v>67336.276297904711</v>
       </c>
-      <c r="C48" s="103">
+      <c r="C48" s="86">
         <f>Calculations!C53</f>
         <v>75409.705751371977</v>
       </c>
-      <c r="D48" s="155">
+      <c r="D48" s="136">
         <f>Calculations!D53</f>
         <v>0.89293912006386023</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="42">
+      <c r="A49" s="37">
         <f>Calculations!A54</f>
         <v>2017</v>
       </c>
-      <c r="B49" s="104">
+      <c r="B49" s="87">
         <f>Calculations!B54</f>
         <v>68138.321384972834</v>
       </c>
-      <c r="C49" s="105">
+      <c r="C49" s="88">
         <f>Calculations!C54</f>
         <v>77294.948395156272</v>
       </c>
-      <c r="D49" s="155"/>
+      <c r="D49" s="136"/>
     </row>
     <row r="50" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
-      <c r="B50" s="73" t="s">
+      <c r="A50" s="27"/>
+      <c r="B50" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="73"/>
-      <c r="D50" s="158">
+      <c r="C50" s="153"/>
+      <c r="D50" s="139">
         <f>Calculations!D55</f>
         <v>0.88153654022288941</v>
       </c>

</xml_diff>